<commit_message>
Updated constraints to include lower bound for leadership
</commit_message>
<xml_diff>
--- a/data/combine_assignments_output/lp_report.xlsx
+++ b/data/combine_assignments_output/lp_report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nickr\Documents\Projects\upwork\carie\UCD LP\data\combine_assignments_output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FB545FE-B5AC-4DCA-B543-41AFADC2021F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85FD13E3-1F70-4F34-AF61-09D8578109B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="30" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pivot" sheetId="2" r:id="rId1"/>
@@ -18,8 +18,8 @@
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="20" r:id="rId3"/>
-    <pivotCache cacheId="25" r:id="rId4"/>
+    <pivotCache cacheId="70" r:id="rId3"/>
+    <pivotCache cacheId="75" r:id="rId4"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -983,28 +983,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1018,7 +997,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Nick Paul" refreshedDate="44784.452078472219" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="102" xr:uid="{F534ADA9-BF7A-4627-85AF-27D4BC27AA15}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Nick Paul" refreshedDate="44805.332623726848" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="102" xr:uid="{F534ADA9-BF7A-4627-85AF-27D4BC27AA15}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:AI1048576" sheet="Data"/>
   </cacheSource>
@@ -1216,7 +1195,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Nick Paul" refreshedDate="44784.452079166665" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="102" xr:uid="{3B7B8082-5ED8-4857-A713-F0A344610BC5}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Nick Paul" refreshedDate="44805.332625000003" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="102" xr:uid="{3B7B8082-5ED8-4857-A713-F0A344610BC5}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:AJ1048576" sheet="Data"/>
   </cacheSource>
@@ -9068,7 +9047,215 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{47850520-E6CC-472F-AE54-FFF027CACE78}" name="PivotTable3" cacheId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{994F79AA-44D0-4A53-8F2D-165FB37F2B53}" name="PivotTable4" cacheId="75" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="Y3:AA28" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="37">
+    <pivotField axis="axisRow" showAll="0" sortType="ascending">
+      <items count="22">
+        <item x="11"/>
+        <item x="8"/>
+        <item x="12"/>
+        <item x="14"/>
+        <item x="9"/>
+        <item x="1"/>
+        <item x="10"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="18"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="0"/>
+        <item x="7"/>
+        <item x="16"/>
+        <item x="15"/>
+        <item x="13"/>
+        <item x="17"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item x="2"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="15">
+        <item x="6"/>
+        <item x="11"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item x="9"/>
+        <item x="4"/>
+        <item x="10"/>
+        <item x="8"/>
+        <item x="12"/>
+        <item x="5"/>
+        <item x="7"/>
+        <item x="0"/>
+        <item x="13"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0">
+      <items count="6">
+        <item n="Other" x="3"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="29"/>
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="25">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i r="1">
+      <x v="8"/>
+    </i>
+    <i r="1">
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="10"/>
+    </i>
+    <i r="1">
+      <x v="11"/>
+    </i>
+    <i r="1">
+      <x v="12"/>
+    </i>
+    <i r="1">
+      <x v="13"/>
+    </i>
+    <i r="1">
+      <x v="14"/>
+    </i>
+    <i r="1">
+      <x v="15"/>
+    </i>
+    <i r="1">
+      <x v="16"/>
+    </i>
+    <i r="1">
+      <x v="17"/>
+    </i>
+    <i r="1">
+      <x v="18"/>
+    </i>
+    <i r="1">
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="20"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of TechSkill" fld="34" baseField="0" baseItem="0"/>
+    <dataField name="Max of Project_Tech_Req" fld="35" subtotal="max" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{47850520-E6CC-472F-AE54-FFF027CACE78}" name="PivotTable3" cacheId="70" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="P3:V29" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="36">
     <pivotField axis="axisRow" showAll="0">
@@ -9286,8 +9473,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{60DF580D-9957-4581-AAEE-DF46E87949C2}" name="PivotTable2" cacheId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{60DF580D-9957-4581-AAEE-DF46E87949C2}" name="PivotTable2" cacheId="70" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="H3:M29" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="36">
     <pivotField axis="axisRow" showAll="0">
@@ -9510,8 +9697,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9C227909-445E-4877-87CE-FC0FA0E0A2FE}" name="PivotTable1" cacheId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9C227909-445E-4877-87CE-FC0FA0E0A2FE}" name="PivotTable1" cacheId="70" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:E29" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="36">
     <pivotField axis="axisRow" showAll="0">
@@ -9718,274 +9905,6 @@
   <dataFields count="1">
     <dataField name="Count of Student_Name" fld="2" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{994F79AA-44D0-4A53-8F2D-165FB37F2B53}" name="PivotTable4" cacheId="25" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="Y3:AA28" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="37">
-    <pivotField axis="axisRow" showAll="0" sortType="ascending">
-      <items count="22">
-        <item x="11"/>
-        <item x="8"/>
-        <item x="12"/>
-        <item x="14"/>
-        <item x="9"/>
-        <item x="1"/>
-        <item x="10"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="18"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="0"/>
-        <item x="7"/>
-        <item x="16"/>
-        <item x="15"/>
-        <item x="13"/>
-        <item x="17"/>
-        <item x="19"/>
-        <item x="20"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item x="2"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="15">
-        <item x="6"/>
-        <item x="11"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item x="9"/>
-        <item x="4"/>
-        <item x="10"/>
-        <item x="8"/>
-        <item x="12"/>
-        <item x="5"/>
-        <item x="7"/>
-        <item x="0"/>
-        <item x="13"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0">
-      <items count="6">
-        <item n="Other" x="3"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item x="4"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="2">
-    <field x="29"/>
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="25">
-    <i>
-      <x/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="4"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i r="1">
-      <x v="7"/>
-    </i>
-    <i r="1">
-      <x v="8"/>
-    </i>
-    <i r="1">
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="10"/>
-    </i>
-    <i r="1">
-      <x v="11"/>
-    </i>
-    <i r="1">
-      <x v="12"/>
-    </i>
-    <i r="1">
-      <x v="13"/>
-    </i>
-    <i r="1">
-      <x v="14"/>
-    </i>
-    <i r="1">
-      <x v="15"/>
-    </i>
-    <i r="1">
-      <x v="16"/>
-    </i>
-    <i r="1">
-      <x v="17"/>
-    </i>
-    <i r="1">
-      <x v="18"/>
-    </i>
-    <i r="1">
-      <x v="19"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="20"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Sum of TechSkill" fld="34" baseField="0" baseItem="0"/>
-    <dataField name="Max of Project_Tech_Req" fld="35" subtotal="max" baseField="0" baseItem="0"/>
-  </dataFields>
-  <conditionalFormats count="1">
-    <conditionalFormat priority="1">
-      <pivotAreas count="3">
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="0" count="10">
-              <x v="0"/>
-              <x v="1"/>
-              <x v="2"/>
-              <x v="3"/>
-              <x v="4"/>
-              <x v="5"/>
-              <x v="6"/>
-              <x v="7"/>
-              <x v="8"/>
-              <x v="9"/>
-            </reference>
-            <reference field="29" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="29" count="1">
-              <x v="1"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="0" count="10">
-              <x v="10"/>
-              <x v="11"/>
-              <x v="12"/>
-              <x v="13"/>
-              <x v="14"/>
-              <x v="15"/>
-              <x v="16"/>
-              <x v="17"/>
-              <x v="18"/>
-              <x v="19"/>
-            </reference>
-            <reference field="29" count="1" selected="0">
-              <x v="1"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-  </conditionalFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -10280,7 +10199,7 @@
   <dimension ref="A2:AA29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="Z6" sqref="Z6"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11733,11 +11652,6 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting pivot="1" sqref="Z5:Z14 Z15 Z16:Z25">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
-      <formula>AA5</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>